<commit_message>
es fr support for -e added
</commit_message>
<xml_diff>
--- a/files/es.xlsx
+++ b/files/es.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20344"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20382"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CABE4AB-3162-46DB-B8B5-1C2F6FB38EF8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12EB5CFF-2BAC-435D-838D-6F3639726CA8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>word</t>
   </si>
@@ -39,83 +39,23 @@
   <si>
     <t>tags</t>
   </si>
-  <si>
-    <t>cobrar?</t>
-  </si>
-  <si>
-    <t>apañar</t>
-  </si>
-  <si>
-    <t>comensales</t>
-  </si>
-  <si>
-    <t>hurtar</t>
-  </si>
-  <si>
-    <t>desprendimiento</t>
-  </si>
-  <si>
-    <t>Großzügigkeit</t>
-  </si>
-  <si>
-    <t>[m]</t>
-  </si>
-  <si>
-    <t>noun</t>
-  </si>
-  <si>
-    <t>muela</t>
-  </si>
-  <si>
-    <t>Backenzahl</t>
-  </si>
-  <si>
-    <t>[f]</t>
-  </si>
-  <si>
-    <t>tachar</t>
-  </si>
-  <si>
-    <t>(aus)streichen, (durch)streichen</t>
-  </si>
-  <si>
-    <t>verb</t>
-  </si>
-  <si>
-    <t>cacahuete</t>
-  </si>
-  <si>
-    <t>tiritas</t>
-  </si>
-  <si>
-    <t>forofo</t>
-  </si>
-  <si>
-    <t>partitura</t>
-  </si>
-  <si>
-    <t>butaca</t>
-  </si>
-  <si>
-    <t>valoración</t>
-  </si>
-  <si>
-    <t>mostaza</t>
-  </si>
-  <si>
-    <t>aspirador</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -160,20 +100,137 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <border outline="0">
         <top style="thin">
           <color indexed="64"/>
         </top>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <border outline="0">
@@ -214,14 +271,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3FF63DEC-5900-4353-8904-279786FCF7D0}" name="Tabelle1" displayName="Tabelle1" ref="A1:E16" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
-  <autoFilter ref="A1:E16" xr:uid="{B1DBE0D5-D96A-41DF-AA0B-B356DE909729}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3FF63DEC-5900-4353-8904-279786FCF7D0}" name="Tabelle1" displayName="Tabelle1" ref="A1:E2" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6">
+  <autoFilter ref="A1:E2" xr:uid="{B1DBE0D5-D96A-41DF-AA0B-B356DE909729}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{13812EEB-F3FB-46C0-9A1B-D7BB29D050E4}" name="word"/>
-    <tableColumn id="2" xr3:uid="{ACFB1A50-7E09-4C61-87B9-EC6DD5A0D268}" name="translation"/>
-    <tableColumn id="3" xr3:uid="{030A37C2-BEE3-423D-8BA2-AD6240871A20}" name="gender"/>
-    <tableColumn id="4" xr3:uid="{4A0EEBB4-8B67-43E0-8033-8A3EC082F661}" name="note"/>
-    <tableColumn id="5" xr3:uid="{CA13EAE9-981F-4AD5-8B02-EB1C27D7D870}" name="tags"/>
+    <tableColumn id="1" xr3:uid="{13812EEB-F3FB-46C0-9A1B-D7BB29D050E4}" name="word" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{ACFB1A50-7E09-4C61-87B9-EC6DD5A0D268}" name="translation" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{030A37C2-BEE3-423D-8BA2-AD6240871A20}" name="gender" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{4A0EEBB4-8B67-43E0-8033-8A3EC082F661}" name="note" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{CA13EAE9-981F-4AD5-8B02-EB1C27D7D870}" name="tags" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -490,16 +547,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" customWidth="1"/>
     <col min="4" max="4" width="19.5703125" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" customWidth="1"/>
@@ -522,106 +579,17 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>26</v>
-      </c>
+    <row r="2" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="5"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>